<commit_message>
test second commit master
</commit_message>
<xml_diff>
--- a/tu vung.xlsx
+++ b/tu vung.xlsx
@@ -2702,7 +2702,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF777777"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2805,7 +2805,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3109,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80:F101"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>

</xml_diff>